<commit_message>
sep 23 70. climbing stairs
</commit_message>
<xml_diff>
--- a/problem notes.xlsx
+++ b/problem notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c0184b455ca2bae/桌面/coding stuff/leetcode repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E37AE8D3-0202-4757-9EFE-87E01B04B177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E37AE8D3-0202-4757-9EFE-87E01B04B177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85966D53-199D-4BA7-B1C3-46C4F4F63856}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="360" windowWidth="19380" windowHeight="10530" xr2:uid="{19F323D1-BE68-418B-840C-C0DF62B72016}"/>
   </bookViews>
@@ -36,13 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>105. Construct Binary Tree from Preorder and Inorder Traversal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>recursive, first index of each subarray of preorder is the root of the subarray. The position of that val in the inorder array shows what nodes is the left child what is right child</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70. Climbing Stairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recursive, DP. 2 ways to get to n step, take 2 step at n - 2, take 1 step at n - 1.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E74C9C-328F-4C4B-96E4-7A1DFDC4CB33}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
@@ -428,8 +436,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
226. Invert Binary Tree
</commit_message>
<xml_diff>
--- a/problem notes.xlsx
+++ b/problem notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c0184b455ca2bae/桌面/coding stuff/leetcode repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{E37AE8D3-0202-4757-9EFE-87E01B04B177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85966D53-199D-4BA7-B1C3-46C4F4F63856}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{E37AE8D3-0202-4757-9EFE-87E01B04B177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47787A1B-FF2C-4351-B4BC-8C62F7959C0F}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="360" windowWidth="19380" windowHeight="10530" xr2:uid="{19F323D1-BE68-418B-840C-C0DF62B72016}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>105. Construct Binary Tree from Preorder and Inorder Traversal</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,22 @@
   </si>
   <si>
     <t>recursive, DP. 2 ways to get to n step, take 2 step at n - 2, take 1 step at n - 1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>322. Coin Change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive, dp, each node returns "least number of coins needed to build its value". At each node take lleast out of all child and + 1 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>238. Product of Array Except Self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make container, populate from left to right and right to left O(2n). Value at each index of container = container[i-1] * nums[i-1]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E74C9C-328F-4C4B-96E4-7A1DFDC4CB33}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
@@ -444,6 +460,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>